<commit_message>
fix: :card_file_box: FIX DATA 2017
</commit_message>
<xml_diff>
--- a/apps/load_data/2017/01/PLMOVMAE.xlsx
+++ b/apps/load_data/2017/01/PLMOVMAE.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NOMBRADOS -2017\HHY0117\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACTUALIZADOS\2017\HHY0117\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3762EF58-3C14-4770-8033-B489EABC7D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645A48E2-CA10-4925-A7A8-0EB39987BAF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLMOVMAE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PLMOVMAE!$A$1:$CF$249</definedName>
     <definedName name="_xlnm.Database">PLMOVMAE!$A$1:$CF$249</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10217" uniqueCount="2482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10205" uniqueCount="2481">
   <si>
     <t>CODEJE</t>
   </si>
@@ -6443,9 +6444,6 @@
   </si>
   <si>
     <t>08771747</t>
-  </si>
-  <si>
-    <t>S/N</t>
   </si>
   <si>
     <t>1047    117305    1173051056     40000     400001081    296920    2969201082    159880    1598802001         0     385992006     38300     383002026    214882    2148822027      3068      30682028      1000         02086      2500         0</t>
@@ -7474,7 +7472,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -8314,10 +8312,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB254" sqref="AB254"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -45455,12 +45455,7 @@
       <c r="AA209" s="1">
         <v>0</v>
       </c>
-      <c r="AC209" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD209" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC209" s="3"/>
       <c r="AF209" s="1" t="s">
         <v>104</v>
       </c>
@@ -45525,10 +45520,10 @@
         <v>112</v>
       </c>
       <c r="BH209" s="1" t="s">
+        <v>2140</v>
+      </c>
+      <c r="BI209" s="1" t="s">
         <v>2141</v>
-      </c>
-      <c r="BI209" s="1" t="s">
-        <v>2142</v>
       </c>
       <c r="BM209" s="1" t="s">
         <v>116</v>
@@ -45537,7 +45532,7 @@
         <v>103</v>
       </c>
       <c r="BT209" s="1" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="BU209" s="1" t="s">
         <v>120</v>
@@ -45558,13 +45553,13 @@
         <v>98</v>
       </c>
       <c r="CC209" s="1" t="s">
+        <v>2143</v>
+      </c>
+      <c r="CD209" s="1" t="s">
         <v>2144</v>
       </c>
-      <c r="CD209" s="1" t="s">
+      <c r="CE209" s="1" t="s">
         <v>2145</v>
-      </c>
-      <c r="CE209" s="1" t="s">
-        <v>2146</v>
       </c>
     </row>
     <row r="210" spans="1:83" x14ac:dyDescent="0.25">
@@ -45599,13 +45594,13 @@
         <v>93</v>
       </c>
       <c r="K210" s="1" t="s">
+        <v>2146</v>
+      </c>
+      <c r="L210" s="1" t="s">
         <v>2147</v>
       </c>
-      <c r="L210" s="1" t="s">
+      <c r="N210" s="1" t="s">
         <v>2148</v>
-      </c>
-      <c r="N210" s="1" t="s">
-        <v>2149</v>
       </c>
       <c r="O210" s="1" t="s">
         <v>97</v>
@@ -45640,12 +45635,7 @@
       <c r="AB210" s="1" t="s">
         <v>1118</v>
       </c>
-      <c r="AC210" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD210" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC210" s="3"/>
       <c r="AF210" s="1" t="s">
         <v>104</v>
       </c>
@@ -45692,7 +45682,7 @@
         <v>98</v>
       </c>
       <c r="AZ210" s="1" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="BB210" s="1">
         <v>1</v>
@@ -45710,10 +45700,10 @@
         <v>112</v>
       </c>
       <c r="BH210" s="1" t="s">
+        <v>2150</v>
+      </c>
+      <c r="BI210" s="1" t="s">
         <v>2151</v>
-      </c>
-      <c r="BI210" s="1" t="s">
-        <v>2152</v>
       </c>
       <c r="BM210" s="1" t="s">
         <v>116</v>
@@ -45725,13 +45715,13 @@
         <v>99</v>
       </c>
       <c r="BR210" s="1" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="BS210" s="3">
         <v>36949</v>
       </c>
       <c r="BT210" s="1" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="BU210" s="1" t="s">
         <v>120</v>
@@ -45755,13 +45745,13 @@
         <v>98</v>
       </c>
       <c r="CC210" s="1" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="CD210" s="1" t="s">
         <v>1780</v>
       </c>
       <c r="CE210" s="1" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="211" spans="1:83" x14ac:dyDescent="0.25">
@@ -45796,13 +45786,13 @@
         <v>93</v>
       </c>
       <c r="K211" s="1" t="s">
+        <v>2156</v>
+      </c>
+      <c r="L211" s="1" t="s">
         <v>2157</v>
       </c>
-      <c r="L211" s="1" t="s">
+      <c r="N211" s="1" t="s">
         <v>2158</v>
-      </c>
-      <c r="N211" s="1" t="s">
-        <v>2159</v>
       </c>
       <c r="O211" s="1" t="s">
         <v>97</v>
@@ -45837,12 +45827,7 @@
       <c r="AB211" s="1" t="s">
         <v>1118</v>
       </c>
-      <c r="AC211" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD211" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC211" s="3"/>
       <c r="AF211" s="1" t="s">
         <v>104</v>
       </c>
@@ -45889,7 +45874,7 @@
         <v>98</v>
       </c>
       <c r="AZ211" s="1" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="BB211" s="1">
         <v>1</v>
@@ -45910,7 +45895,7 @@
         <v>112</v>
       </c>
       <c r="BH211" s="1" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="BI211" s="1" t="s">
         <v>1447</v>
@@ -45925,13 +45910,13 @@
         <v>99</v>
       </c>
       <c r="BR211" s="1" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="BS211" s="3">
         <v>36825</v>
       </c>
       <c r="BT211" s="1" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="BU211" s="1" t="s">
         <v>120</v>
@@ -45955,13 +45940,13 @@
         <v>98</v>
       </c>
       <c r="CC211" s="1" t="s">
+        <v>2163</v>
+      </c>
+      <c r="CD211" s="1" t="s">
         <v>2164</v>
       </c>
-      <c r="CD211" s="1" t="s">
+      <c r="CE211" s="1" t="s">
         <v>2165</v>
-      </c>
-      <c r="CE211" s="1" t="s">
-        <v>2166</v>
       </c>
     </row>
     <row r="212" spans="1:83" x14ac:dyDescent="0.25">
@@ -45996,13 +45981,13 @@
         <v>93</v>
       </c>
       <c r="K212" s="1" t="s">
+        <v>2166</v>
+      </c>
+      <c r="L212" s="1" t="s">
         <v>2167</v>
       </c>
-      <c r="L212" s="1" t="s">
+      <c r="N212" s="1" t="s">
         <v>2168</v>
-      </c>
-      <c r="N212" s="1" t="s">
-        <v>2169</v>
       </c>
       <c r="O212" s="1" t="s">
         <v>97</v>
@@ -46034,12 +46019,7 @@
       <c r="AA212" s="1">
         <v>0</v>
       </c>
-      <c r="AC212" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD212" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC212" s="3"/>
       <c r="AF212" s="1" t="s">
         <v>104</v>
       </c>
@@ -46089,7 +46069,7 @@
         <v>98</v>
       </c>
       <c r="AZ212" s="1" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="BB212" s="1">
         <v>1</v>
@@ -46107,7 +46087,7 @@
         <v>112</v>
       </c>
       <c r="BH212" s="1" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="BI212" s="1" t="s">
         <v>179</v>
@@ -46119,7 +46099,7 @@
         <v>103</v>
       </c>
       <c r="BT212" s="1" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="BU212" s="1" t="s">
         <v>120</v>
@@ -46137,13 +46117,13 @@
         <v>98</v>
       </c>
       <c r="CC212" s="1" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="CD212" s="1" t="s">
         <v>1103</v>
       </c>
       <c r="CE212" s="1" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="213" spans="1:83" x14ac:dyDescent="0.25">
@@ -46178,13 +46158,13 @@
         <v>93</v>
       </c>
       <c r="K213" s="1" t="s">
+        <v>2174</v>
+      </c>
+      <c r="L213" s="1" t="s">
         <v>2175</v>
       </c>
-      <c r="L213" s="1" t="s">
+      <c r="N213" s="1" t="s">
         <v>2176</v>
-      </c>
-      <c r="N213" s="1" t="s">
-        <v>2177</v>
       </c>
       <c r="O213" s="1" t="s">
         <v>97</v>
@@ -46216,12 +46196,7 @@
       <c r="AA213" s="1">
         <v>0</v>
       </c>
-      <c r="AC213" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD213" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC213" s="3"/>
       <c r="AF213" s="1" t="s">
         <v>104</v>
       </c>
@@ -46271,7 +46246,7 @@
         <v>98</v>
       </c>
       <c r="AZ213" s="1" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="BB213" s="1">
         <v>1</v>
@@ -46289,7 +46264,7 @@
         <v>112</v>
       </c>
       <c r="BH213" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="BI213" s="1" t="s">
         <v>621</v>
@@ -46301,7 +46276,7 @@
         <v>103</v>
       </c>
       <c r="BT213" s="1" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="BU213" s="1" t="s">
         <v>120</v>
@@ -46322,10 +46297,10 @@
         <v>645</v>
       </c>
       <c r="CD213" s="1" t="s">
+        <v>2180</v>
+      </c>
+      <c r="CE213" s="1" t="s">
         <v>2181</v>
-      </c>
-      <c r="CE213" s="1" t="s">
-        <v>2182</v>
       </c>
     </row>
     <row r="214" spans="1:83" x14ac:dyDescent="0.25">
@@ -46360,13 +46335,13 @@
         <v>93</v>
       </c>
       <c r="K214" s="1" t="s">
+        <v>2182</v>
+      </c>
+      <c r="L214" s="1" t="s">
         <v>2183</v>
       </c>
-      <c r="L214" s="1" t="s">
+      <c r="N214" s="1" t="s">
         <v>2184</v>
-      </c>
-      <c r="N214" s="1" t="s">
-        <v>2185</v>
       </c>
       <c r="O214" s="1" t="s">
         <v>97</v>
@@ -46398,12 +46373,7 @@
       <c r="AA214" s="1">
         <v>0</v>
       </c>
-      <c r="AC214" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD214" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC214" s="3"/>
       <c r="AF214" s="1" t="s">
         <v>104</v>
       </c>
@@ -46453,7 +46423,7 @@
         <v>98</v>
       </c>
       <c r="AZ214" s="1" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="BB214" s="1">
         <v>1</v>
@@ -46474,7 +46444,7 @@
         <v>928</v>
       </c>
       <c r="BI214" s="1" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="BM214" s="1" t="s">
         <v>116</v>
@@ -46483,7 +46453,7 @@
         <v>103</v>
       </c>
       <c r="BT214" s="1" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="BU214" s="1" t="s">
         <v>120</v>
@@ -46501,13 +46471,13 @@
         <v>98</v>
       </c>
       <c r="CC214" s="1" t="s">
+        <v>2188</v>
+      </c>
+      <c r="CD214" s="1" t="s">
+        <v>2188</v>
+      </c>
+      <c r="CE214" s="1" t="s">
         <v>2189</v>
-      </c>
-      <c r="CD214" s="1" t="s">
-        <v>2189</v>
-      </c>
-      <c r="CE214" s="1" t="s">
-        <v>2190</v>
       </c>
     </row>
     <row r="215" spans="1:83" x14ac:dyDescent="0.25">
@@ -46542,13 +46512,13 @@
         <v>93</v>
       </c>
       <c r="K215" s="1" t="s">
+        <v>2190</v>
+      </c>
+      <c r="L215" s="1" t="s">
         <v>2191</v>
       </c>
-      <c r="L215" s="1" t="s">
+      <c r="N215" s="1" t="s">
         <v>2192</v>
-      </c>
-      <c r="N215" s="1" t="s">
-        <v>2193</v>
       </c>
       <c r="O215" s="1" t="s">
         <v>97</v>
@@ -46586,12 +46556,7 @@
       <c r="AA215" s="1">
         <v>0</v>
       </c>
-      <c r="AC215" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD215" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC215" s="3"/>
       <c r="AF215" s="1" t="s">
         <v>104</v>
       </c>
@@ -46638,7 +46603,7 @@
         <v>98</v>
       </c>
       <c r="AZ215" s="1" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="BB215" s="1">
         <v>1</v>
@@ -46647,7 +46612,7 @@
         <v>17</v>
       </c>
       <c r="BD215" s="1" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="BE215" s="1" t="s">
         <v>110</v>
@@ -46659,7 +46624,7 @@
         <v>112</v>
       </c>
       <c r="BH215" s="1" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="BI215" s="1" t="s">
         <v>255</v>
@@ -46674,13 +46639,13 @@
         <v>117</v>
       </c>
       <c r="BR215" s="1" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="BS215" s="3">
         <v>35243</v>
       </c>
       <c r="BT215" s="1" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="BU215" s="1" t="s">
         <v>120</v>
@@ -46698,13 +46663,13 @@
         <v>98</v>
       </c>
       <c r="CC215" s="1" t="s">
+        <v>2198</v>
+      </c>
+      <c r="CD215" s="1" t="s">
         <v>2199</v>
       </c>
-      <c r="CD215" s="1" t="s">
+      <c r="CE215" s="1" t="s">
         <v>2200</v>
-      </c>
-      <c r="CE215" s="1" t="s">
-        <v>2201</v>
       </c>
     </row>
     <row r="216" spans="1:83" x14ac:dyDescent="0.25">
@@ -46739,13 +46704,13 @@
         <v>93</v>
       </c>
       <c r="K216" s="1" t="s">
+        <v>2201</v>
+      </c>
+      <c r="L216" s="1" t="s">
         <v>2202</v>
       </c>
-      <c r="L216" s="1" t="s">
+      <c r="N216" s="1" t="s">
         <v>2203</v>
-      </c>
-      <c r="N216" s="1" t="s">
-        <v>2204</v>
       </c>
       <c r="O216" s="1" t="s">
         <v>97</v>
@@ -46777,12 +46742,7 @@
       <c r="AA216" s="1">
         <v>0</v>
       </c>
-      <c r="AC216" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD216" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC216" s="3"/>
       <c r="AF216" s="1" t="s">
         <v>104</v>
       </c>
@@ -46832,7 +46792,7 @@
         <v>98</v>
       </c>
       <c r="AZ216" s="1" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="BB216" s="1">
         <v>1</v>
@@ -46850,7 +46810,7 @@
         <v>112</v>
       </c>
       <c r="BH216" s="1" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="BI216" s="1" t="s">
         <v>2089</v>
@@ -46862,7 +46822,7 @@
         <v>103</v>
       </c>
       <c r="BT216" s="1" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="BU216" s="1" t="s">
         <v>120</v>
@@ -46880,13 +46840,13 @@
         <v>98</v>
       </c>
       <c r="CC216" s="1" t="s">
+        <v>2207</v>
+      </c>
+      <c r="CD216" s="1" t="s">
         <v>2208</v>
       </c>
-      <c r="CD216" s="1" t="s">
+      <c r="CE216" s="1" t="s">
         <v>2209</v>
-      </c>
-      <c r="CE216" s="1" t="s">
-        <v>2210</v>
       </c>
     </row>
     <row r="217" spans="1:83" x14ac:dyDescent="0.25">
@@ -46921,13 +46881,13 @@
         <v>93</v>
       </c>
       <c r="K217" s="1" t="s">
+        <v>2210</v>
+      </c>
+      <c r="L217" s="1" t="s">
         <v>2211</v>
       </c>
-      <c r="L217" s="1" t="s">
+      <c r="N217" s="1" t="s">
         <v>2212</v>
-      </c>
-      <c r="N217" s="1" t="s">
-        <v>2213</v>
       </c>
       <c r="O217" s="1" t="s">
         <v>97</v>
@@ -46959,12 +46919,7 @@
       <c r="AA217" s="1">
         <v>0</v>
       </c>
-      <c r="AC217" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD217" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC217" s="3"/>
       <c r="AF217" s="1" t="s">
         <v>104</v>
       </c>
@@ -47014,7 +46969,7 @@
         <v>98</v>
       </c>
       <c r="AZ217" s="1" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="BB217" s="1">
         <v>1</v>
@@ -47032,10 +46987,10 @@
         <v>112</v>
       </c>
       <c r="BH217" s="1" t="s">
+        <v>2214</v>
+      </c>
+      <c r="BI217" s="1" t="s">
         <v>2215</v>
-      </c>
-      <c r="BI217" s="1" t="s">
-        <v>2216</v>
       </c>
       <c r="BM217" s="1" t="s">
         <v>116</v>
@@ -47047,7 +47002,7 @@
         <v>155</v>
       </c>
       <c r="BT217" s="1" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="BU217" s="1" t="s">
         <v>120</v>
@@ -47065,13 +47020,13 @@
         <v>98</v>
       </c>
       <c r="CC217" s="1" t="s">
+        <v>2217</v>
+      </c>
+      <c r="CD217" s="1" t="s">
         <v>2218</v>
       </c>
-      <c r="CD217" s="1" t="s">
+      <c r="CE217" s="1" t="s">
         <v>2219</v>
-      </c>
-      <c r="CE217" s="1" t="s">
-        <v>2220</v>
       </c>
     </row>
     <row r="218" spans="1:83" x14ac:dyDescent="0.25">
@@ -47106,13 +47061,13 @@
         <v>93</v>
       </c>
       <c r="K218" s="1" t="s">
+        <v>2220</v>
+      </c>
+      <c r="L218" s="1" t="s">
         <v>2221</v>
       </c>
-      <c r="L218" s="1" t="s">
+      <c r="N218" s="1" t="s">
         <v>2222</v>
-      </c>
-      <c r="N218" s="1" t="s">
-        <v>2223</v>
       </c>
       <c r="O218" s="1" t="s">
         <v>97</v>
@@ -47144,12 +47099,7 @@
       <c r="AA218" s="1">
         <v>0</v>
       </c>
-      <c r="AC218" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD218" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC218" s="3"/>
       <c r="AF218" s="1" t="s">
         <v>104</v>
       </c>
@@ -47196,7 +47146,7 @@
         <v>98</v>
       </c>
       <c r="AZ218" s="1" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="BB218" s="1">
         <v>1</v>
@@ -47205,7 +47155,7 @@
         <v>17</v>
       </c>
       <c r="BD218" s="1" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="BE218" s="1" t="s">
         <v>110</v>
@@ -47217,10 +47167,10 @@
         <v>112</v>
       </c>
       <c r="BH218" s="1" t="s">
+        <v>2225</v>
+      </c>
+      <c r="BI218" s="1" t="s">
         <v>2226</v>
-      </c>
-      <c r="BI218" s="1" t="s">
-        <v>2227</v>
       </c>
       <c r="BM218" s="1" t="s">
         <v>116</v>
@@ -47232,13 +47182,13 @@
         <v>207</v>
       </c>
       <c r="BR218" s="1" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="BS218" s="3">
         <v>34307</v>
       </c>
       <c r="BT218" s="1" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="BU218" s="1" t="s">
         <v>120</v>
@@ -47256,13 +47206,13 @@
         <v>98</v>
       </c>
       <c r="CC218" s="1" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="CD218" s="1" t="s">
         <v>427</v>
       </c>
       <c r="CE218" s="1" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="219" spans="1:83" x14ac:dyDescent="0.25">
@@ -47297,13 +47247,13 @@
         <v>93</v>
       </c>
       <c r="K219" s="1" t="s">
+        <v>2231</v>
+      </c>
+      <c r="L219" s="1" t="s">
         <v>2232</v>
       </c>
-      <c r="L219" s="1" t="s">
+      <c r="N219" s="1" t="s">
         <v>2233</v>
-      </c>
-      <c r="N219" s="1" t="s">
-        <v>2234</v>
       </c>
       <c r="O219" s="1" t="s">
         <v>97</v>
@@ -47338,12 +47288,7 @@
       <c r="AA219" s="1">
         <v>0</v>
       </c>
-      <c r="AC219" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD219" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC219" s="3"/>
       <c r="AF219" s="1" t="s">
         <v>104</v>
       </c>
@@ -47393,7 +47338,7 @@
         <v>98</v>
       </c>
       <c r="AZ219" s="1" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="BB219" s="1">
         <v>1</v>
@@ -47414,10 +47359,10 @@
         <v>112</v>
       </c>
       <c r="BH219" s="1" t="s">
+        <v>2235</v>
+      </c>
+      <c r="BI219" s="1" t="s">
         <v>2236</v>
-      </c>
-      <c r="BI219" s="1" t="s">
-        <v>2237</v>
       </c>
       <c r="BM219" s="1" t="s">
         <v>116</v>
@@ -47426,7 +47371,7 @@
         <v>103</v>
       </c>
       <c r="BT219" s="1" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="BU219" s="1" t="s">
         <v>120</v>
@@ -47447,13 +47392,13 @@
         <v>98</v>
       </c>
       <c r="CC219" s="1" t="s">
+        <v>2238</v>
+      </c>
+      <c r="CD219" s="1" t="s">
         <v>2239</v>
       </c>
-      <c r="CD219" s="1" t="s">
+      <c r="CE219" s="1" t="s">
         <v>2240</v>
-      </c>
-      <c r="CE219" s="1" t="s">
-        <v>2241</v>
       </c>
     </row>
     <row r="220" spans="1:83" x14ac:dyDescent="0.25">
@@ -47488,13 +47433,13 @@
         <v>93</v>
       </c>
       <c r="K220" s="1" t="s">
+        <v>2241</v>
+      </c>
+      <c r="L220" s="1" t="s">
         <v>2242</v>
       </c>
-      <c r="L220" s="1" t="s">
+      <c r="N220" s="1" t="s">
         <v>2243</v>
-      </c>
-      <c r="N220" s="1" t="s">
-        <v>2244</v>
       </c>
       <c r="O220" s="1" t="s">
         <v>97</v>
@@ -47526,12 +47471,7 @@
       <c r="AA220" s="1">
         <v>0</v>
       </c>
-      <c r="AC220" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD220" s="1" t="s">
-        <v>2140</v>
-      </c>
+      <c r="AC220" s="3"/>
       <c r="AF220" s="1" t="s">
         <v>104</v>
       </c>
@@ -47578,7 +47518,7 @@
         <v>98</v>
       </c>
       <c r="AZ220" s="1" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
       <c r="BB220" s="1">
         <v>1</v>
@@ -47599,10 +47539,10 @@
         <v>112</v>
       </c>
       <c r="BH220" s="1" t="s">
+        <v>2245</v>
+      </c>
+      <c r="BI220" s="1" t="s">
         <v>2246</v>
-      </c>
-      <c r="BI220" s="1" t="s">
-        <v>2247</v>
       </c>
       <c r="BM220" s="1" t="s">
         <v>116</v>
@@ -47614,13 +47554,13 @@
         <v>117</v>
       </c>
       <c r="BR220" s="1" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
       <c r="BS220" s="3">
         <v>35950</v>
       </c>
       <c r="BT220" s="1" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
       <c r="BU220" s="1" t="s">
         <v>120</v>
@@ -47638,13 +47578,13 @@
         <v>98</v>
       </c>
       <c r="CC220" s="1" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
       <c r="CD220" s="1" t="s">
         <v>1610</v>
       </c>
       <c r="CE220" s="1" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="221" spans="1:83" x14ac:dyDescent="0.25">
@@ -47679,13 +47619,13 @@
         <v>317</v>
       </c>
       <c r="K221" s="1" t="s">
+        <v>2251</v>
+      </c>
+      <c r="L221" s="1" t="s">
         <v>2252</v>
       </c>
-      <c r="L221" s="1" t="s">
+      <c r="N221" s="1" t="s">
         <v>2253</v>
-      </c>
-      <c r="N221" s="1" t="s">
-        <v>2254</v>
       </c>
       <c r="O221" s="1" t="s">
         <v>97</v>
@@ -47736,7 +47676,7 @@
         <v>0</v>
       </c>
       <c r="AN221" s="1" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="AO221" s="1">
         <v>0</v>
@@ -47781,13 +47721,13 @@
         <v>112</v>
       </c>
       <c r="BH221" s="1" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="BM221" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BT221" s="1" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
       <c r="BU221" s="1" t="s">
         <v>120</v>
@@ -47811,10 +47751,10 @@
         <v>2040</v>
       </c>
       <c r="CD221" s="1" t="s">
+        <v>2257</v>
+      </c>
+      <c r="CE221" s="1" t="s">
         <v>2258</v>
-      </c>
-      <c r="CE221" s="1" t="s">
-        <v>2259</v>
       </c>
     </row>
     <row r="222" spans="1:83" x14ac:dyDescent="0.25">
@@ -47849,13 +47789,13 @@
         <v>317</v>
       </c>
       <c r="K222" s="1" t="s">
+        <v>2259</v>
+      </c>
+      <c r="L222" s="1" t="s">
         <v>2260</v>
       </c>
-      <c r="L222" s="1" t="s">
+      <c r="N222" s="1" t="s">
         <v>2261</v>
-      </c>
-      <c r="N222" s="1" t="s">
-        <v>2262</v>
       </c>
       <c r="O222" s="1" t="s">
         <v>97</v>
@@ -47909,7 +47849,7 @@
         <v>0</v>
       </c>
       <c r="AN222" s="1" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="AO222" s="1">
         <v>0</v>
@@ -47954,13 +47894,13 @@
         <v>112</v>
       </c>
       <c r="BH222" s="1" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="BM222" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BT222" s="1" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
       <c r="BU222" s="1" t="s">
         <v>120</v>
@@ -47981,13 +47921,13 @@
         <v>98</v>
       </c>
       <c r="CC222" s="1" t="s">
+        <v>2264</v>
+      </c>
+      <c r="CD222" s="1" t="s">
         <v>2265</v>
       </c>
-      <c r="CD222" s="1" t="s">
+      <c r="CE222" s="1" t="s">
         <v>2266</v>
-      </c>
-      <c r="CE222" s="1" t="s">
-        <v>2267</v>
       </c>
     </row>
     <row r="223" spans="1:83" x14ac:dyDescent="0.25">
@@ -48022,13 +47962,13 @@
         <v>317</v>
       </c>
       <c r="K223" s="1" t="s">
+        <v>2267</v>
+      </c>
+      <c r="L223" s="1" t="s">
         <v>2268</v>
       </c>
-      <c r="L223" s="1" t="s">
+      <c r="N223" s="1" t="s">
         <v>2269</v>
-      </c>
-      <c r="N223" s="1" t="s">
-        <v>2270</v>
       </c>
       <c r="O223" s="1" t="s">
         <v>97</v>
@@ -48082,7 +48022,7 @@
         <v>0</v>
       </c>
       <c r="AN223" s="1" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="AO223" s="1">
         <v>0</v>
@@ -48127,13 +48067,13 @@
         <v>112</v>
       </c>
       <c r="BH223" s="1" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
       <c r="BM223" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BT223" s="1" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="BU223" s="1" t="s">
         <v>120</v>
@@ -48154,13 +48094,13 @@
         <v>98</v>
       </c>
       <c r="CC223" s="1" t="s">
+        <v>2272</v>
+      </c>
+      <c r="CD223" s="1" t="s">
         <v>2273</v>
       </c>
-      <c r="CD223" s="1" t="s">
+      <c r="CE223" s="1" t="s">
         <v>2274</v>
-      </c>
-      <c r="CE223" s="1" t="s">
-        <v>2275</v>
       </c>
     </row>
     <row r="224" spans="1:83" x14ac:dyDescent="0.25">
@@ -48195,13 +48135,13 @@
         <v>317</v>
       </c>
       <c r="K224" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="L224" s="1" t="s">
         <v>2276</v>
       </c>
-      <c r="L224" s="1" t="s">
+      <c r="N224" s="1" t="s">
         <v>2277</v>
-      </c>
-      <c r="N224" s="1" t="s">
-        <v>2278</v>
       </c>
       <c r="O224" s="1" t="s">
         <v>97</v>
@@ -48297,13 +48237,13 @@
         <v>112</v>
       </c>
       <c r="BH224" s="1" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="BM224" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BT224" s="1" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="BU224" s="1" t="s">
         <v>120</v>
@@ -48324,10 +48264,10 @@
         <v>98</v>
       </c>
       <c r="CC224" s="1" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="CD224" s="1" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="CE224" s="1" t="s">
         <v>195</v>
@@ -48365,13 +48305,13 @@
         <v>317</v>
       </c>
       <c r="K225" s="1" t="s">
+        <v>2281</v>
+      </c>
+      <c r="L225" s="1" t="s">
         <v>2282</v>
       </c>
-      <c r="L225" s="1" t="s">
+      <c r="N225" s="1" t="s">
         <v>2283</v>
-      </c>
-      <c r="N225" s="1" t="s">
-        <v>2284</v>
       </c>
       <c r="O225" s="1" t="s">
         <v>97</v>
@@ -48425,7 +48365,7 @@
         <v>0</v>
       </c>
       <c r="AN225" s="1" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="AO225" s="1">
         <v>0</v>
@@ -48470,13 +48410,13 @@
         <v>112</v>
       </c>
       <c r="BH225" s="1" t="s">
-        <v>2285</v>
+        <v>2284</v>
       </c>
       <c r="BM225" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BT225" s="1" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
       <c r="BU225" s="1" t="s">
         <v>120</v>
@@ -48500,13 +48440,13 @@
         <v>98</v>
       </c>
       <c r="CC225" s="1" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="CD225" s="1" t="s">
         <v>1126</v>
       </c>
       <c r="CE225" s="1" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="226" spans="1:83" x14ac:dyDescent="0.25">
@@ -48541,13 +48481,13 @@
         <v>317</v>
       </c>
       <c r="K226" s="1" t="s">
+        <v>2288</v>
+      </c>
+      <c r="L226" s="1" t="s">
         <v>2289</v>
       </c>
-      <c r="L226" s="1" t="s">
+      <c r="N226" s="1" t="s">
         <v>2290</v>
-      </c>
-      <c r="N226" s="1" t="s">
-        <v>2291</v>
       </c>
       <c r="O226" s="1" t="s">
         <v>97</v>
@@ -48598,7 +48538,7 @@
         <v>0</v>
       </c>
       <c r="AN226" s="1" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="AO226" s="1">
         <v>0</v>
@@ -48643,13 +48583,13 @@
         <v>112</v>
       </c>
       <c r="BH226" s="1" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="BM226" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BT226" s="1" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="BU226" s="1" t="s">
         <v>120</v>
@@ -48670,13 +48610,13 @@
         <v>98</v>
       </c>
       <c r="CC226" s="1" t="s">
+        <v>2294</v>
+      </c>
+      <c r="CD226" s="1" t="s">
+        <v>2208</v>
+      </c>
+      <c r="CE226" s="1" t="s">
         <v>2295</v>
-      </c>
-      <c r="CD226" s="1" t="s">
-        <v>2209</v>
-      </c>
-      <c r="CE226" s="1" t="s">
-        <v>2296</v>
       </c>
     </row>
     <row r="227" spans="1:83" x14ac:dyDescent="0.25">
@@ -48711,10 +48651,10 @@
         <v>93</v>
       </c>
       <c r="K227" s="1" t="s">
+        <v>2296</v>
+      </c>
+      <c r="L227" s="1" t="s">
         <v>2297</v>
-      </c>
-      <c r="L227" s="1" t="s">
-        <v>2298</v>
       </c>
       <c r="O227" s="1" t="s">
         <v>97</v>
@@ -48783,7 +48723,7 @@
         <v>16</v>
       </c>
       <c r="BD227" s="1" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="BX227" s="1">
         <v>0</v>
@@ -48801,7 +48741,7 @@
         <v>221</v>
       </c>
       <c r="CE227" s="1" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="228" spans="1:83" x14ac:dyDescent="0.25">
@@ -48836,10 +48776,10 @@
         <v>93</v>
       </c>
       <c r="K228" s="1" t="s">
+        <v>2299</v>
+      </c>
+      <c r="L228" s="1" t="s">
         <v>2300</v>
-      </c>
-      <c r="L228" s="1" t="s">
-        <v>2301</v>
       </c>
       <c r="O228" s="1" t="s">
         <v>97</v>
@@ -48923,7 +48863,7 @@
         <v>221</v>
       </c>
       <c r="CE228" s="1" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="229" spans="1:83" x14ac:dyDescent="0.25">
@@ -48958,13 +48898,13 @@
         <v>93</v>
       </c>
       <c r="K229" s="1" t="s">
+        <v>2301</v>
+      </c>
+      <c r="L229" s="1" t="s">
         <v>2302</v>
       </c>
-      <c r="L229" s="1" t="s">
+      <c r="N229" s="1" t="s">
         <v>2303</v>
-      </c>
-      <c r="N229" s="1" t="s">
-        <v>2304</v>
       </c>
       <c r="O229" s="1" t="s">
         <v>97</v>
@@ -49045,7 +48985,7 @@
         <v>98</v>
       </c>
       <c r="AZ229" s="1" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="BB229" s="1">
         <v>1</v>
@@ -49063,10 +49003,10 @@
         <v>112</v>
       </c>
       <c r="BH229" s="1" t="s">
+        <v>2305</v>
+      </c>
+      <c r="BI229" s="1" t="s">
         <v>2306</v>
-      </c>
-      <c r="BI229" s="1" t="s">
-        <v>2307</v>
       </c>
       <c r="BM229" s="1" t="s">
         <v>116</v>
@@ -49078,7 +49018,7 @@
         <v>155</v>
       </c>
       <c r="BT229" s="1" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="BU229" s="1" t="s">
         <v>120</v>
@@ -49096,13 +49036,13 @@
         <v>98</v>
       </c>
       <c r="CC229" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="CD229" s="1" t="s">
         <v>427</v>
       </c>
       <c r="CE229" s="1" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="230" spans="1:83" x14ac:dyDescent="0.25">
@@ -49137,13 +49077,13 @@
         <v>93</v>
       </c>
       <c r="K230" s="1" t="s">
+        <v>2310</v>
+      </c>
+      <c r="L230" s="1" t="s">
         <v>2311</v>
       </c>
-      <c r="L230" s="1" t="s">
+      <c r="N230" s="1" t="s">
         <v>2312</v>
-      </c>
-      <c r="N230" s="1" t="s">
-        <v>2313</v>
       </c>
       <c r="O230" s="1" t="s">
         <v>97</v>
@@ -49221,7 +49161,7 @@
         <v>98</v>
       </c>
       <c r="AZ230" s="1" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="BB230" s="1">
         <v>1</v>
@@ -49239,10 +49179,10 @@
         <v>112</v>
       </c>
       <c r="BH230" s="1" t="s">
+        <v>2314</v>
+      </c>
+      <c r="BI230" s="1" t="s">
         <v>2315</v>
-      </c>
-      <c r="BI230" s="1" t="s">
-        <v>2316</v>
       </c>
       <c r="BM230" s="1" t="s">
         <v>116</v>
@@ -49254,13 +49194,13 @@
         <v>207</v>
       </c>
       <c r="BR230" s="1" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="BS230" s="3">
         <v>36099</v>
       </c>
       <c r="BT230" s="1" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="BU230" s="1" t="s">
         <v>120</v>
@@ -49278,13 +49218,13 @@
         <v>98</v>
       </c>
       <c r="CC230" s="1" t="s">
+        <v>2318</v>
+      </c>
+      <c r="CD230" s="1" t="s">
         <v>2319</v>
       </c>
-      <c r="CD230" s="1" t="s">
+      <c r="CE230" s="1" t="s">
         <v>2320</v>
-      </c>
-      <c r="CE230" s="1" t="s">
-        <v>2321</v>
       </c>
     </row>
     <row r="231" spans="1:83" x14ac:dyDescent="0.25">
@@ -49319,13 +49259,13 @@
         <v>93</v>
       </c>
       <c r="K231" s="1" t="s">
+        <v>2321</v>
+      </c>
+      <c r="L231" s="1" t="s">
         <v>2322</v>
       </c>
-      <c r="L231" s="1" t="s">
+      <c r="N231" s="1" t="s">
         <v>2323</v>
-      </c>
-      <c r="N231" s="1" t="s">
-        <v>2324</v>
       </c>
       <c r="O231" s="1" t="s">
         <v>97</v>
@@ -49403,7 +49343,7 @@
         <v>98</v>
       </c>
       <c r="AZ231" s="1" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="BB231" s="1">
         <v>1</v>
@@ -49421,10 +49361,10 @@
         <v>112</v>
       </c>
       <c r="BH231" s="1" t="s">
+        <v>2325</v>
+      </c>
+      <c r="BI231" s="1" t="s">
         <v>2326</v>
-      </c>
-      <c r="BI231" s="1" t="s">
-        <v>2327</v>
       </c>
       <c r="BM231" s="1" t="s">
         <v>116</v>
@@ -49436,13 +49376,13 @@
         <v>99</v>
       </c>
       <c r="BR231" s="1" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="BS231" s="3">
         <v>37735</v>
       </c>
       <c r="BT231" s="1" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="BU231" s="1" t="s">
         <v>120</v>
@@ -49460,13 +49400,13 @@
         <v>98</v>
       </c>
       <c r="CC231" s="1" t="s">
+        <v>2329</v>
+      </c>
+      <c r="CD231" s="1" t="s">
         <v>2330</v>
       </c>
-      <c r="CD231" s="1" t="s">
+      <c r="CE231" s="1" t="s">
         <v>2331</v>
-      </c>
-      <c r="CE231" s="1" t="s">
-        <v>2332</v>
       </c>
     </row>
     <row r="232" spans="1:83" x14ac:dyDescent="0.25">
@@ -49501,13 +49441,13 @@
         <v>93</v>
       </c>
       <c r="K232" s="1" t="s">
+        <v>2332</v>
+      </c>
+      <c r="L232" s="1" t="s">
         <v>2333</v>
       </c>
-      <c r="L232" s="1" t="s">
+      <c r="N232" s="1" t="s">
         <v>2334</v>
-      </c>
-      <c r="N232" s="1" t="s">
-        <v>2335</v>
       </c>
       <c r="O232" s="1" t="s">
         <v>97</v>
@@ -49588,7 +49528,7 @@
         <v>98</v>
       </c>
       <c r="AZ232" s="1" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="BB232" s="1">
         <v>1</v>
@@ -49606,10 +49546,10 @@
         <v>112</v>
       </c>
       <c r="BH232" s="1" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="BI232" s="1" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="BM232" s="1" t="s">
         <v>116</v>
@@ -49618,7 +49558,7 @@
         <v>103</v>
       </c>
       <c r="BT232" s="1" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="BU232" s="1" t="s">
         <v>120</v>
@@ -49636,13 +49576,13 @@
         <v>98</v>
       </c>
       <c r="CC232" s="1" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="CD232" s="1" t="s">
         <v>805</v>
       </c>
       <c r="CE232" s="1" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="233" spans="1:83" x14ac:dyDescent="0.25">
@@ -49677,13 +49617,13 @@
         <v>93</v>
       </c>
       <c r="K233" s="1" t="s">
+        <v>2340</v>
+      </c>
+      <c r="L233" s="1" t="s">
         <v>2341</v>
       </c>
-      <c r="L233" s="1" t="s">
+      <c r="N233" s="1" t="s">
         <v>2342</v>
-      </c>
-      <c r="N233" s="1" t="s">
-        <v>2343</v>
       </c>
       <c r="O233" s="1" t="s">
         <v>97</v>
@@ -49719,7 +49659,7 @@
         <v>104</v>
       </c>
       <c r="AG233" s="1" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="AH233" s="1" t="s">
         <v>1716</v>
@@ -49764,7 +49704,7 @@
         <v>98</v>
       </c>
       <c r="AZ233" s="1" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="BB233" s="1">
         <v>1</v>
@@ -49782,7 +49722,7 @@
         <v>112</v>
       </c>
       <c r="BH233" s="1" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="BI233" s="1" t="s">
         <v>2080</v>
@@ -49794,7 +49734,7 @@
         <v>103</v>
       </c>
       <c r="BT233" s="1" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="BU233" s="1" t="s">
         <v>120</v>
@@ -49815,10 +49755,10 @@
         <v>1428</v>
       </c>
       <c r="CD233" s="1" t="s">
+        <v>2347</v>
+      </c>
+      <c r="CE233" s="1" t="s">
         <v>2348</v>
-      </c>
-      <c r="CE233" s="1" t="s">
-        <v>2349</v>
       </c>
     </row>
     <row r="234" spans="1:83" x14ac:dyDescent="0.25">
@@ -49853,13 +49793,13 @@
         <v>93</v>
       </c>
       <c r="K234" s="1" t="s">
+        <v>2349</v>
+      </c>
+      <c r="L234" s="1" t="s">
         <v>2350</v>
       </c>
-      <c r="L234" s="1" t="s">
+      <c r="N234" s="1" t="s">
         <v>2351</v>
-      </c>
-      <c r="N234" s="1" t="s">
-        <v>2352</v>
       </c>
       <c r="O234" s="1" t="s">
         <v>97</v>
@@ -49940,7 +49880,7 @@
         <v>98</v>
       </c>
       <c r="AZ234" s="1" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="BB234" s="1">
         <v>1</v>
@@ -49958,10 +49898,10 @@
         <v>112</v>
       </c>
       <c r="BH234" s="1" t="s">
+        <v>2353</v>
+      </c>
+      <c r="BI234" s="1" t="s">
         <v>2354</v>
-      </c>
-      <c r="BI234" s="1" t="s">
-        <v>2355</v>
       </c>
       <c r="BM234" s="1" t="s">
         <v>116</v>
@@ -49970,7 +49910,7 @@
         <v>103</v>
       </c>
       <c r="BT234" s="1" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="BU234" s="1" t="s">
         <v>120</v>
@@ -49994,7 +49934,7 @@
         <v>871</v>
       </c>
       <c r="CE234" s="1" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="235" spans="1:83" x14ac:dyDescent="0.25">
@@ -50029,13 +49969,13 @@
         <v>93</v>
       </c>
       <c r="K235" s="1" t="s">
+        <v>2357</v>
+      </c>
+      <c r="L235" s="1" t="s">
         <v>2358</v>
       </c>
-      <c r="L235" s="1" t="s">
+      <c r="N235" s="1" t="s">
         <v>2359</v>
-      </c>
-      <c r="N235" s="1" t="s">
-        <v>2360</v>
       </c>
       <c r="O235" s="1" t="s">
         <v>97</v>
@@ -50074,7 +50014,7 @@
         <v>618</v>
       </c>
       <c r="AH235" s="1" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="AI235" s="1" t="s">
         <v>98</v>
@@ -50116,7 +50056,7 @@
         <v>98</v>
       </c>
       <c r="AZ235" s="1" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="BB235" s="1">
         <v>1</v>
@@ -50134,10 +50074,10 @@
         <v>112</v>
       </c>
       <c r="BH235" s="1" t="s">
+        <v>2362</v>
+      </c>
+      <c r="BI235" s="1" t="s">
         <v>2363</v>
-      </c>
-      <c r="BI235" s="1" t="s">
-        <v>2364</v>
       </c>
       <c r="BM235" s="1" t="s">
         <v>116</v>
@@ -50146,7 +50086,7 @@
         <v>103</v>
       </c>
       <c r="BT235" s="1" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="BU235" s="1" t="s">
         <v>120</v>
@@ -50164,13 +50104,13 @@
         <v>98</v>
       </c>
       <c r="CC235" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="CD235" s="1" t="s">
         <v>2366</v>
       </c>
-      <c r="CD235" s="1" t="s">
+      <c r="CE235" s="1" t="s">
         <v>2367</v>
-      </c>
-      <c r="CE235" s="1" t="s">
-        <v>2368</v>
       </c>
     </row>
     <row r="236" spans="1:83" x14ac:dyDescent="0.25">
@@ -50205,13 +50145,13 @@
         <v>317</v>
       </c>
       <c r="K236" s="1" t="s">
+        <v>2368</v>
+      </c>
+      <c r="L236" s="1" t="s">
         <v>2369</v>
       </c>
-      <c r="L236" s="1" t="s">
+      <c r="N236" s="1" t="s">
         <v>2370</v>
-      </c>
-      <c r="N236" s="1" t="s">
-        <v>2371</v>
       </c>
       <c r="O236" s="1" t="s">
         <v>97</v>
@@ -50253,7 +50193,7 @@
         <v>0</v>
       </c>
       <c r="AN236" s="1" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="AO236" s="1">
         <v>0</v>
@@ -50292,13 +50232,13 @@
         <v>112</v>
       </c>
       <c r="BH236" s="1" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="BM236" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BT236" s="1" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="BU236" s="1" t="s">
         <v>120</v>
@@ -50316,13 +50256,13 @@
         <v>98</v>
       </c>
       <c r="CC236" s="1" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="CD236" s="1" t="s">
         <v>299</v>
       </c>
       <c r="CE236" s="1" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="237" spans="1:83" x14ac:dyDescent="0.25">
@@ -50357,13 +50297,13 @@
         <v>93</v>
       </c>
       <c r="K237" s="1" t="s">
+        <v>2376</v>
+      </c>
+      <c r="L237" s="1" t="s">
         <v>2377</v>
       </c>
-      <c r="L237" s="1" t="s">
+      <c r="N237" s="1" t="s">
         <v>2378</v>
-      </c>
-      <c r="N237" s="1" t="s">
-        <v>2379</v>
       </c>
       <c r="O237" s="1" t="s">
         <v>97</v>
@@ -50405,7 +50345,7 @@
         <v>42247</v>
       </c>
       <c r="AD237" s="1" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="AF237" s="1" t="s">
         <v>104</v>
@@ -50459,7 +50399,7 @@
         <v>17</v>
       </c>
       <c r="BD237" s="1" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="BE237" s="1" t="s">
         <v>110</v>
@@ -50471,10 +50411,10 @@
         <v>112</v>
       </c>
       <c r="BH237" s="1" t="s">
+        <v>2380</v>
+      </c>
+      <c r="BI237" s="1" t="s">
         <v>2381</v>
-      </c>
-      <c r="BI237" s="1" t="s">
-        <v>2382</v>
       </c>
       <c r="BM237" s="1" t="s">
         <v>116</v>
@@ -50486,13 +50426,13 @@
         <v>207</v>
       </c>
       <c r="BR237" s="1" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="BS237" s="3">
         <v>36580</v>
       </c>
       <c r="BT237" s="1" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="BU237" s="1" t="s">
         <v>120</v>
@@ -50513,7 +50453,7 @@
         <v>98</v>
       </c>
       <c r="CC237" s="1" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="CD237" s="1" t="s">
         <v>287</v>
@@ -50554,13 +50494,13 @@
         <v>93</v>
       </c>
       <c r="K238" s="1" t="s">
+        <v>2385</v>
+      </c>
+      <c r="L238" s="1" t="s">
         <v>2386</v>
       </c>
-      <c r="L238" s="1" t="s">
+      <c r="N238" s="1" t="s">
         <v>2387</v>
-      </c>
-      <c r="N238" s="1" t="s">
-        <v>2388</v>
       </c>
       <c r="O238" s="1" t="s">
         <v>97</v>
@@ -50656,7 +50596,7 @@
         <v>112</v>
       </c>
       <c r="BH238" s="1" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="BI238" s="1" t="s">
         <v>2080</v>
@@ -50671,13 +50611,13 @@
         <v>117</v>
       </c>
       <c r="BR238" s="1" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="BS238" s="3">
         <v>37747</v>
       </c>
       <c r="BT238" s="1" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="BU238" s="1" t="s">
         <v>120</v>
@@ -50701,7 +50641,7 @@
         <v>635</v>
       </c>
       <c r="CE238" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="239" spans="1:83" x14ac:dyDescent="0.25">
@@ -50736,13 +50676,13 @@
         <v>93</v>
       </c>
       <c r="K239" s="1" t="s">
+        <v>2392</v>
+      </c>
+      <c r="L239" s="1" t="s">
         <v>2393</v>
       </c>
-      <c r="L239" s="1" t="s">
+      <c r="N239" s="1" t="s">
         <v>2394</v>
-      </c>
-      <c r="N239" s="1" t="s">
-        <v>2395</v>
       </c>
       <c r="O239" s="1" t="s">
         <v>97</v>
@@ -50838,7 +50778,7 @@
         <v>112</v>
       </c>
       <c r="BH239" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="BM239" s="1" t="s">
         <v>116</v>
@@ -50847,7 +50787,7 @@
         <v>103</v>
       </c>
       <c r="BT239" s="1" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="BU239" s="1" t="s">
         <v>120</v>
@@ -50865,13 +50805,13 @@
         <v>98</v>
       </c>
       <c r="CC239" s="1" t="s">
+        <v>2397</v>
+      </c>
+      <c r="CD239" s="1" t="s">
         <v>2398</v>
       </c>
-      <c r="CD239" s="1" t="s">
+      <c r="CE239" s="1" t="s">
         <v>2399</v>
-      </c>
-      <c r="CE239" s="1" t="s">
-        <v>2400</v>
       </c>
     </row>
     <row r="240" spans="1:83" x14ac:dyDescent="0.25">
@@ -50906,13 +50846,13 @@
         <v>93</v>
       </c>
       <c r="K240" s="1" t="s">
+        <v>2400</v>
+      </c>
+      <c r="L240" s="1" t="s">
         <v>2401</v>
       </c>
-      <c r="L240" s="1" t="s">
+      <c r="N240" s="1" t="s">
         <v>2402</v>
-      </c>
-      <c r="N240" s="1" t="s">
-        <v>2403</v>
       </c>
       <c r="O240" s="1" t="s">
         <v>97</v>
@@ -50951,7 +50891,7 @@
         <v>618</v>
       </c>
       <c r="AH240" s="1" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="AI240" s="1" t="s">
         <v>98</v>
@@ -51008,10 +50948,10 @@
         <v>112</v>
       </c>
       <c r="BH240" s="1" t="s">
+        <v>2403</v>
+      </c>
+      <c r="BI240" s="1" t="s">
         <v>2404</v>
-      </c>
-      <c r="BI240" s="1" t="s">
-        <v>2405</v>
       </c>
       <c r="BM240" s="1" t="s">
         <v>116</v>
@@ -51020,7 +50960,7 @@
         <v>103</v>
       </c>
       <c r="BT240" s="1" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="BU240" s="1" t="s">
         <v>120</v>
@@ -51038,13 +50978,13 @@
         <v>98</v>
       </c>
       <c r="CC240" s="1" t="s">
+        <v>2406</v>
+      </c>
+      <c r="CD240" s="1" t="s">
         <v>2407</v>
       </c>
-      <c r="CD240" s="1" t="s">
+      <c r="CE240" s="1" t="s">
         <v>2408</v>
-      </c>
-      <c r="CE240" s="1" t="s">
-        <v>2409</v>
       </c>
     </row>
     <row r="241" spans="1:83" x14ac:dyDescent="0.25">
@@ -51079,13 +51019,13 @@
         <v>93</v>
       </c>
       <c r="K241" s="1" t="s">
+        <v>2409</v>
+      </c>
+      <c r="L241" s="1" t="s">
         <v>2410</v>
       </c>
-      <c r="L241" s="1" t="s">
+      <c r="N241" s="1" t="s">
         <v>2411</v>
-      </c>
-      <c r="N241" s="1" t="s">
-        <v>2412</v>
       </c>
       <c r="O241" s="1" t="s">
         <v>97</v>
@@ -51124,7 +51064,7 @@
         <v>618</v>
       </c>
       <c r="AH241" s="1" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="AJ241" s="1" t="s">
         <v>107</v>
@@ -51181,10 +51121,10 @@
         <v>112</v>
       </c>
       <c r="BH241" s="1" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="BI241" s="1" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="BM241" s="1" t="s">
         <v>116</v>
@@ -51196,13 +51136,13 @@
         <v>99</v>
       </c>
       <c r="BR241" s="1" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="BS241" s="3">
         <v>37334</v>
       </c>
       <c r="BT241" s="1" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="BU241" s="1" t="s">
         <v>120</v>
@@ -51223,10 +51163,10 @@
         <v>510</v>
       </c>
       <c r="CD241" s="1" t="s">
+        <v>2415</v>
+      </c>
+      <c r="CE241" s="1" t="s">
         <v>2416</v>
-      </c>
-      <c r="CE241" s="1" t="s">
-        <v>2417</v>
       </c>
     </row>
     <row r="242" spans="1:83" x14ac:dyDescent="0.25">
@@ -51261,13 +51201,13 @@
         <v>93</v>
       </c>
       <c r="K242" s="1" t="s">
+        <v>2417</v>
+      </c>
+      <c r="L242" s="1" t="s">
         <v>2418</v>
       </c>
-      <c r="L242" s="1" t="s">
+      <c r="N242" s="1" t="s">
         <v>2419</v>
-      </c>
-      <c r="N242" s="1" t="s">
-        <v>2420</v>
       </c>
       <c r="O242" s="1" t="s">
         <v>97</v>
@@ -51363,7 +51303,7 @@
         <v>112</v>
       </c>
       <c r="BH242" s="1" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="BI242" s="1" t="s">
         <v>1872</v>
@@ -51378,13 +51318,13 @@
         <v>99</v>
       </c>
       <c r="BR242" s="1" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="BS242" s="3">
         <v>37904</v>
       </c>
       <c r="BT242" s="1" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="BU242" s="1" t="s">
         <v>120</v>
@@ -51405,10 +51345,10 @@
         <v>871</v>
       </c>
       <c r="CD242" s="1" t="s">
+        <v>2423</v>
+      </c>
+      <c r="CE242" s="1" t="s">
         <v>2424</v>
-      </c>
-      <c r="CE242" s="1" t="s">
-        <v>2425</v>
       </c>
     </row>
     <row r="243" spans="1:83" x14ac:dyDescent="0.25">
@@ -51443,13 +51383,13 @@
         <v>93</v>
       </c>
       <c r="K243" s="1" t="s">
+        <v>2425</v>
+      </c>
+      <c r="L243" s="1" t="s">
         <v>2426</v>
       </c>
-      <c r="L243" s="1" t="s">
+      <c r="N243" s="1" t="s">
         <v>2427</v>
-      </c>
-      <c r="N243" s="1" t="s">
-        <v>2428</v>
       </c>
       <c r="O243" s="1" t="s">
         <v>97</v>
@@ -51542,7 +51482,7 @@
         <v>112</v>
       </c>
       <c r="BH243" s="1" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="BM243" s="1" t="s">
         <v>116</v>
@@ -51554,13 +51494,13 @@
         <v>117</v>
       </c>
       <c r="BR243" s="1" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="BS243" s="3">
         <v>36111</v>
       </c>
       <c r="BT243" s="1" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="BU243" s="1" t="s">
         <v>120</v>
@@ -51578,13 +51518,13 @@
         <v>98</v>
       </c>
       <c r="CC243" s="1" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="CD243" s="1" t="s">
         <v>1028</v>
       </c>
       <c r="CE243" s="1" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="244" spans="1:83" x14ac:dyDescent="0.25">
@@ -51619,13 +51559,13 @@
         <v>93</v>
       </c>
       <c r="K244" s="1" t="s">
+        <v>2433</v>
+      </c>
+      <c r="L244" s="1" t="s">
         <v>2434</v>
       </c>
-      <c r="L244" s="1" t="s">
+      <c r="N244" s="1" t="s">
         <v>2435</v>
-      </c>
-      <c r="N244" s="1" t="s">
-        <v>2436</v>
       </c>
       <c r="O244" s="1" t="s">
         <v>97</v>
@@ -51721,7 +51661,7 @@
         <v>112</v>
       </c>
       <c r="BH244" s="1" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="BI244" s="1" t="s">
         <v>1666</v>
@@ -51736,13 +51676,13 @@
         <v>117</v>
       </c>
       <c r="BR244" s="1" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="BS244" s="3">
         <v>37785</v>
       </c>
       <c r="BT244" s="1" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="BU244" s="1" t="s">
         <v>120</v>
@@ -51760,13 +51700,13 @@
         <v>98</v>
       </c>
       <c r="CC244" s="1" t="s">
+        <v>2439</v>
+      </c>
+      <c r="CD244" s="1" t="s">
         <v>2440</v>
       </c>
-      <c r="CD244" s="1" t="s">
+      <c r="CE244" s="1" t="s">
         <v>2441</v>
-      </c>
-      <c r="CE244" s="1" t="s">
-        <v>2442</v>
       </c>
     </row>
     <row r="245" spans="1:83" x14ac:dyDescent="0.25">
@@ -51801,13 +51741,13 @@
         <v>93</v>
       </c>
       <c r="K245" s="1" t="s">
+        <v>2442</v>
+      </c>
+      <c r="L245" s="1" t="s">
         <v>2443</v>
       </c>
-      <c r="L245" s="1" t="s">
+      <c r="N245" s="1" t="s">
         <v>2444</v>
-      </c>
-      <c r="N245" s="1" t="s">
-        <v>2445</v>
       </c>
       <c r="O245" s="1" t="s">
         <v>97</v>
@@ -51903,7 +51843,7 @@
         <v>112</v>
       </c>
       <c r="BH245" s="1" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="BM245" s="1" t="s">
         <v>116</v>
@@ -51912,7 +51852,7 @@
         <v>103</v>
       </c>
       <c r="BT245" s="1" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="BU245" s="1" t="s">
         <v>120</v>
@@ -51933,10 +51873,10 @@
         <v>1140</v>
       </c>
       <c r="CD245" s="1" t="s">
+        <v>2447</v>
+      </c>
+      <c r="CE245" s="1" t="s">
         <v>2448</v>
-      </c>
-      <c r="CE245" s="1" t="s">
-        <v>2449</v>
       </c>
     </row>
     <row r="246" spans="1:83" x14ac:dyDescent="0.25">
@@ -51974,10 +51914,10 @@
         <v>249</v>
       </c>
       <c r="L246" s="1" t="s">
+        <v>2449</v>
+      </c>
+      <c r="M246" s="1" t="s">
         <v>2450</v>
-      </c>
-      <c r="M246" s="1" t="s">
-        <v>2451</v>
       </c>
       <c r="N246" s="1" t="s">
         <v>251</v>
@@ -52010,7 +51950,7 @@
         <v>42582</v>
       </c>
       <c r="AD246" s="1" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="AF246" s="1" t="s">
         <v>104</v>
@@ -52061,10 +52001,10 @@
         <v>252</v>
       </c>
       <c r="BH246" s="1" t="s">
+        <v>2452</v>
+      </c>
+      <c r="BI246" s="1" t="s">
         <v>2453</v>
-      </c>
-      <c r="BI246" s="1" t="s">
-        <v>2454</v>
       </c>
       <c r="BM246" s="1" t="s">
         <v>116</v>
@@ -52138,16 +52078,16 @@
         <v>93</v>
       </c>
       <c r="K247" s="1" t="s">
+        <v>2454</v>
+      </c>
+      <c r="L247" s="1" t="s">
         <v>2455</v>
       </c>
-      <c r="L247" s="1" t="s">
+      <c r="M247" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="N247" s="1" t="s">
         <v>2456</v>
-      </c>
-      <c r="M247" s="1" t="s">
-        <v>2451</v>
-      </c>
-      <c r="N247" s="1" t="s">
-        <v>2457</v>
       </c>
       <c r="Q247" s="3">
         <v>17060</v>
@@ -52183,7 +52123,7 @@
         <v>42628</v>
       </c>
       <c r="AD247" s="1" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="AF247" s="1" t="s">
         <v>104</v>
@@ -52234,16 +52174,16 @@
         <v>98</v>
       </c>
       <c r="AZ247" s="1" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="BD247" s="1" t="s">
         <v>219</v>
       </c>
       <c r="BH247" s="1" t="s">
+        <v>2459</v>
+      </c>
+      <c r="BI247" s="1" t="s">
         <v>2460</v>
-      </c>
-      <c r="BI247" s="1" t="s">
-        <v>2461</v>
       </c>
       <c r="BM247" s="1" t="s">
         <v>116</v>
@@ -52252,7 +52192,7 @@
         <v>103</v>
       </c>
       <c r="BT247" s="1" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="BU247" s="1" t="s">
         <v>120</v>
@@ -52276,7 +52216,7 @@
         <v>124</v>
       </c>
       <c r="CE247" s="1" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="248" spans="1:83" x14ac:dyDescent="0.25">
@@ -52311,16 +52251,16 @@
         <v>93</v>
       </c>
       <c r="K248" s="1" t="s">
+        <v>2463</v>
+      </c>
+      <c r="L248" s="1" t="s">
         <v>2464</v>
       </c>
-      <c r="L248" s="1" t="s">
+      <c r="M248" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="N248" s="1" t="s">
         <v>2465</v>
-      </c>
-      <c r="M248" s="1" t="s">
-        <v>2451</v>
-      </c>
-      <c r="N248" s="1" t="s">
-        <v>2466</v>
       </c>
       <c r="Q248" s="3">
         <v>26864</v>
@@ -52350,7 +52290,7 @@
         <v>42735</v>
       </c>
       <c r="AD248" s="1" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="AF248" s="1" t="s">
         <v>104</v>
@@ -52401,7 +52341,7 @@
         <v>99</v>
       </c>
       <c r="BH248" s="1" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="BM248" s="1" t="s">
         <v>116</v>
@@ -52413,13 +52353,13 @@
         <v>207</v>
       </c>
       <c r="BR248" s="1" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="BS248" s="3">
         <v>102</v>
       </c>
       <c r="BT248" s="1" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="BU248" s="1" t="s">
         <v>120</v>
@@ -52440,13 +52380,13 @@
         <v>98</v>
       </c>
       <c r="CC248" s="1" t="s">
+        <v>2470</v>
+      </c>
+      <c r="CD248" s="1" t="s">
         <v>2471</v>
       </c>
-      <c r="CD248" s="1" t="s">
+      <c r="CE248" s="1" t="s">
         <v>2472</v>
-      </c>
-      <c r="CE248" s="1" t="s">
-        <v>2473</v>
       </c>
     </row>
     <row r="249" spans="1:83" x14ac:dyDescent="0.25">
@@ -52481,16 +52421,16 @@
         <v>93</v>
       </c>
       <c r="K249" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="L249" s="1" t="s">
         <v>2474</v>
       </c>
-      <c r="L249" s="1" t="s">
+      <c r="M249" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="N249" s="1" t="s">
         <v>2475</v>
-      </c>
-      <c r="M249" s="1" t="s">
-        <v>2451</v>
-      </c>
-      <c r="N249" s="1" t="s">
-        <v>2476</v>
       </c>
       <c r="Q249" s="3">
         <v>17041</v>
@@ -52517,7 +52457,7 @@
         <v>42735</v>
       </c>
       <c r="AD249" s="1" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="AF249" s="1" t="s">
         <v>104</v>
@@ -52568,7 +52508,7 @@
         <v>98</v>
       </c>
       <c r="BH249" s="1" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="BM249" s="1" t="s">
         <v>116</v>
@@ -52577,7 +52517,7 @@
         <v>103</v>
       </c>
       <c r="BT249" s="1" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="BU249" s="1" t="s">
         <v>120</v>
@@ -52598,16 +52538,17 @@
         <v>98</v>
       </c>
       <c r="CC249" s="1" t="s">
+        <v>2478</v>
+      </c>
+      <c r="CD249" s="1" t="s">
         <v>2479</v>
       </c>
-      <c r="CD249" s="1" t="s">
+      <c r="CE249" s="1" t="s">
         <v>2480</v>
-      </c>
-      <c r="CE249" s="1" t="s">
-        <v>2481</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:CF249" xr:uid="{CACE21CC-DE0E-475A-A784-29311B77C758}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>